<commit_message>
day 32 - mammamia finished
</commit_message>
<xml_diff>
--- a/AndroidStudio/Proyecto Final/mammamia/puntuacion/Rúbrica Proyectos PMDM.xlsx
+++ b/AndroidStudio/Proyecto Final/mammamia/puntuacion/Rúbrica Proyectos PMDM.xlsx
@@ -92,7 +92,7 @@
   </si>
   <si>
     <t xml:space="preserve">Persistencia
-Si sólo se implmentá guardado en preferencias =&gt; Bajo
+Si sólo se implementa guardado en preferencias =&gt; Bajo
 SQLite o Firebase =&gt; Medio o alto en función de la lógica
 SQLite y Firebase =&gt; Alto</t>
   </si>
@@ -535,10 +535,10 @@
   <dimension ref="B1:Q998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.75"/>

</xml_diff>